<commit_message>
refactor data gathering steps
</commit_message>
<xml_diff>
--- a/timeline.xlsx
+++ b/timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\adityamahesa\productivities\self-project\py-thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F45416-2C48-4053-AA5F-F741881FB0DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6D3DEA-83AA-4E0A-9603-868701B43AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{02874B45-5096-4E7C-B905-DAF755EAD9C2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="67">
   <si>
     <t>code</t>
   </si>
@@ -205,6 +205,36 @@
   </si>
   <si>
     <t>2023-08-01</t>
+  </si>
+  <si>
+    <t>scraping_end_date</t>
+  </si>
+  <si>
+    <t>2019-07-25</t>
+  </si>
+  <si>
+    <t>2019-08-15</t>
+  </si>
+  <si>
+    <t>2019-10-14</t>
+  </si>
+  <si>
+    <t>2019-11-12</t>
+  </si>
+  <si>
+    <t>scraping_start_date</t>
+  </si>
+  <si>
+    <t>2020-12-29</t>
+  </si>
+  <si>
+    <t>2022-11-04</t>
+  </si>
+  <si>
+    <t>2022-12-06</t>
+  </si>
+  <si>
+    <t>2023-06-12</t>
   </si>
 </sst>
 </file>
@@ -571,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C06105B6-E61B-4C6B-BC93-0C314FE22FA4}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,9 +616,11 @@
     <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -613,8 +645,14 @@
       <c r="H1" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -639,8 +677,14 @@
       <c r="H2" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -665,8 +709,14 @@
       <c r="H3" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -691,8 +741,14 @@
       <c r="H4" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -717,8 +773,14 @@
       <c r="H5" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -743,8 +805,14 @@
       <c r="H6" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -769,8 +837,14 @@
       <c r="H7" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -795,8 +869,14 @@
       <c r="H8" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
@@ -821,11 +901,17 @@
       <c r="H9" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D11" s="1"/>
     </row>
   </sheetData>

</xml_diff>